<commit_message>
Updated .bib file to fix formatting errors, Ch. 1
.bib file had formatting errors, style errors
Ch. 1 - minor revisions
</commit_message>
<xml_diff>
--- a/Appendix1/chv-reports-2013.xlsx
+++ b/Appendix1/chv-reports-2013.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Pregnant women</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>Indicator</t>
+  </si>
+  <si>
+    <t>Homes visited</t>
+  </si>
+  <si>
+    <t>Number per month (1/2013-6/2013)</t>
+  </si>
+  <si>
+    <t>Number per month (7/2013-3/2014)</t>
+  </si>
+  <si>
+    <t>Total number (1/2013-6/2013)</t>
+  </si>
+  <si>
+    <t>Total number (7/2013-3/2014)</t>
   </si>
 </sst>
 </file>
@@ -130,11 +145,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,18 +455,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A13" sqref="A13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.28515625" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -473,7 +493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -500,8 +520,16 @@
         <f>SUM(B2:G2)</f>
         <v>1414</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>H2/6</f>
+        <v>235.66666666666666</v>
+      </c>
+      <c r="J2">
+        <f>95/6</f>
+        <v>15.833333333333334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -528,7 +556,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -555,7 +583,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -582,7 +610,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -609,7 +637,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -635,8 +663,16 @@
         <f t="shared" si="0"/>
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f>172/6</f>
+        <v>28.666666666666668</v>
+      </c>
+      <c r="J7">
+        <f>71/8</f>
+        <v>8.875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -663,7 +699,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -690,7 +726,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -717,7 +753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -742,6 +778,118 @@
       <c r="H11">
         <f t="shared" si="0"/>
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>236</v>
+      </c>
+      <c r="C14" s="5">
+        <f>G14/8</f>
+        <v>11.875</v>
+      </c>
+      <c r="F14">
+        <v>1414</v>
+      </c>
+      <c r="G14">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5">
+        <f>F15/6</f>
+        <v>28.666666666666668</v>
+      </c>
+      <c r="C15" s="5">
+        <f>G15/8</f>
+        <v>8.875</v>
+      </c>
+      <c r="F15">
+        <v>172</v>
+      </c>
+      <c r="G15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1414</v>
+      </c>
+      <c r="C20">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>95</v>
+      </c>
+      <c r="C21">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>236</v>
+      </c>
+      <c r="C22" s="5">
+        <f>C20/6</f>
+        <v>28.666666666666668</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5">
+        <f>B21/8</f>
+        <v>11.875</v>
+      </c>
+      <c r="C23" s="5">
+        <f>C21/8</f>
+        <v>8.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>